<commit_message>
mental health am initial commit
</commit_message>
<xml_diff>
--- a/Senior Centers MySidewalk Profiles/Update Log.xlsx
+++ b/Senior Centers MySidewalk Profiles/Update Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmccall\Documents\GIT\Aging-and-Disability\Senior Centers MySidewalk Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED97233-9F6B-46B6-A0C7-9451C14CBAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1954DC-725C-4C29-875C-50F239B725DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{940324B9-2625-4B70-BB57-73308F3561E9}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="126">
   <si>
     <t>Center</t>
   </si>
@@ -350,10 +349,70 @@
     <t>65-68</t>
   </si>
   <si>
-    <t>pop density not showing up</t>
-  </si>
-  <si>
     <t>https://reports.mysidewalk.com/89727cd83b</t>
+  </si>
+  <si>
+    <t>Sharing Link</t>
+  </si>
+  <si>
+    <t>Map Notes</t>
+  </si>
+  <si>
+    <t>some maps small pop</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/9c98ac8d7f</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/d56badf939</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/182f8c30d9</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/d7c6c60790</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/25e533510f</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/aa88bfc635</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/d9dc823ab0</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/62c6ab6c49</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/402a7f85c8</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/abe29aba06</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/6d3597601c</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/12f00466ee</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/de97ba31bb</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/ab9b517d33</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/6029acb213</t>
+  </si>
+  <si>
+    <t>https://reports.mysidewalk.com/1f9c415316</t>
+  </si>
+  <si>
+    <t>ajax</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -721,22 +780,25 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="44.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="27.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -773,6 +835,15 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
+      <c r="M1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -814,6 +885,9 @@
       <c r="M2" t="s">
         <v>86</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -834,6 +908,12 @@
       <c r="F3" t="s">
         <v>66</v>
       </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
       <c r="I3" t="s">
         <v>83</v>
       </c>
@@ -848,6 +928,12 @@
       </c>
       <c r="M3" t="s">
         <v>86</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="O3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -869,6 +955,12 @@
       <c r="F4" t="s">
         <v>67</v>
       </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
       <c r="I4" t="s">
         <v>83</v>
       </c>
@@ -883,6 +975,12 @@
       </c>
       <c r="M4" t="s">
         <v>85</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -904,6 +1002,12 @@
       <c r="F5" t="s">
         <v>68</v>
       </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
       <c r="I5" t="s">
         <v>83</v>
       </c>
@@ -918,6 +1022,12 @@
       </c>
       <c r="M5" t="s">
         <v>86</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="O5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -939,6 +1049,12 @@
       <c r="F6" t="s">
         <v>69</v>
       </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
       <c r="I6" t="s">
         <v>83</v>
       </c>
@@ -953,6 +1069,12 @@
       </c>
       <c r="M6" t="s">
         <v>84</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -974,6 +1096,12 @@
       <c r="F7" t="s">
         <v>70</v>
       </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
       <c r="I7" t="s">
         <v>83</v>
       </c>
@@ -988,6 +1116,12 @@
       </c>
       <c r="M7" t="s">
         <v>86</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="O7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1009,6 +1143,12 @@
       <c r="F8" t="s">
         <v>65</v>
       </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" t="s">
         <v>83</v>
       </c>
@@ -1023,6 +1163,12 @@
       </c>
       <c r="M8" t="s">
         <v>86</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="O8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1044,6 +1190,12 @@
       <c r="F9" t="s">
         <v>72</v>
       </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
       <c r="I9" t="s">
         <v>83</v>
       </c>
@@ -1055,6 +1207,15 @@
       </c>
       <c r="L9" t="s">
         <v>83</v>
+      </c>
+      <c r="M9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="O9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1076,6 +1237,12 @@
       <c r="F10" t="s">
         <v>78</v>
       </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
       <c r="I10" t="s">
         <v>83</v>
       </c>
@@ -1088,8 +1255,14 @@
       <c r="L10" t="s">
         <v>83</v>
       </c>
-      <c r="N10" t="s">
-        <v>104</v>
+      <c r="M10" t="s">
+        <v>86</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="O10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1111,6 +1284,12 @@
       <c r="F11" t="s">
         <v>71</v>
       </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
       <c r="I11" t="s">
         <v>83</v>
       </c>
@@ -1123,8 +1302,14 @@
       <c r="L11" t="s">
         <v>83</v>
       </c>
-      <c r="N11" t="s">
-        <v>104</v>
+      <c r="M11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1146,6 +1331,12 @@
       <c r="F12" t="s">
         <v>73</v>
       </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
       <c r="I12" t="s">
         <v>83</v>
       </c>
@@ -1157,6 +1348,15 @@
       </c>
       <c r="L12" t="s">
         <v>83</v>
+      </c>
+      <c r="M12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O12" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1178,6 +1378,12 @@
       <c r="F13" t="s">
         <v>74</v>
       </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
       <c r="I13" t="s">
         <v>83</v>
       </c>
@@ -1189,6 +1395,15 @@
       </c>
       <c r="L13" t="s">
         <v>83</v>
+      </c>
+      <c r="M13" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="O13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1210,6 +1425,12 @@
       <c r="F14" t="s">
         <v>75</v>
       </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
       <c r="I14" t="s">
         <v>83</v>
       </c>
@@ -1221,6 +1442,15 @@
       </c>
       <c r="L14" t="s">
         <v>83</v>
+      </c>
+      <c r="M14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="O14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1242,6 +1472,12 @@
       <c r="F15" t="s">
         <v>80</v>
       </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
       <c r="I15" t="s">
         <v>83</v>
       </c>
@@ -1253,6 +1489,15 @@
       </c>
       <c r="L15" t="s">
         <v>83</v>
+      </c>
+      <c r="M15" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O15" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1274,6 +1519,12 @@
       <c r="F16" t="s">
         <v>76</v>
       </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
       <c r="I16" t="s">
         <v>83</v>
       </c>
@@ -1287,13 +1538,16 @@
         <v>83</v>
       </c>
       <c r="M16" t="s">
-        <v>85</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="O16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>102</v>
       </c>
@@ -1312,6 +1566,12 @@
       <c r="F17" t="s">
         <v>77</v>
       </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
       <c r="I17" t="s">
         <v>83</v>
       </c>
@@ -1324,8 +1584,17 @@
       <c r="L17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>86</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>103</v>
       </c>
@@ -1344,6 +1613,12 @@
       <c r="F18" t="s">
         <v>79</v>
       </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
       <c r="I18" t="s">
         <v>83</v>
       </c>
@@ -1355,11 +1630,36 @@
       </c>
       <c r="L18" t="s">
         <v>83</v>
+      </c>
+      <c r="M18" t="s">
+        <v>86</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="O18" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O16" r:id="rId1" xr:uid="{3C51300E-85D2-40F7-A07F-40C478F5519B}"/>
+    <hyperlink ref="N16" r:id="rId1" xr:uid="{3C51300E-85D2-40F7-A07F-40C478F5519B}"/>
+    <hyperlink ref="N2" r:id="rId2" xr:uid="{9B528625-E1D3-4A00-8C3F-F8A6302F3D80}"/>
+    <hyperlink ref="N3" r:id="rId3" xr:uid="{72FD0191-0BEF-4122-8F27-E35B58E93977}"/>
+    <hyperlink ref="N4" r:id="rId4" xr:uid="{6ED45E4E-C287-4E07-B7F2-7004829683E6}"/>
+    <hyperlink ref="N5" r:id="rId5" xr:uid="{D88AEC80-4AD8-4785-81D7-C4B9D073E90C}"/>
+    <hyperlink ref="N6" r:id="rId6" xr:uid="{31E5EA3A-927A-4611-8902-F4137E264A60}"/>
+    <hyperlink ref="N7" r:id="rId7" xr:uid="{275923B3-D9EA-46CA-9F30-FB9FE2C3802D}"/>
+    <hyperlink ref="N8" r:id="rId8" xr:uid="{E4421F06-4829-4138-9DFE-05B62D58326B}"/>
+    <hyperlink ref="N9" r:id="rId9" xr:uid="{DB3BC50E-FAD2-4BA6-9B03-58324BFD74EA}"/>
+    <hyperlink ref="N10" r:id="rId10" xr:uid="{45489982-45E2-4E4A-A7B1-A8BE17315679}"/>
+    <hyperlink ref="N11" r:id="rId11" xr:uid="{D4FFBE38-805E-48FE-8F82-991287E62B62}"/>
+    <hyperlink ref="N12" r:id="rId12" xr:uid="{E8D1FDC2-3526-4D38-9F1D-87ABE1297838}"/>
+    <hyperlink ref="N13" r:id="rId13" xr:uid="{A74D715D-AE46-469F-9215-9E08B048BFCD}"/>
+    <hyperlink ref="N14" r:id="rId14" xr:uid="{3675F322-FA47-442D-B0C3-4C805141FE50}"/>
+    <hyperlink ref="N15" r:id="rId15" xr:uid="{F1832BE1-5B60-4830-B015-A5A452314E8C}"/>
+    <hyperlink ref="N17" r:id="rId16" xr:uid="{14F61905-BF13-4925-818D-2FB7E074FF77}"/>
+    <hyperlink ref="N18" r:id="rId17" xr:uid="{A045B208-595D-4E74-BD30-2CE4E3243D86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>